<commit_message>
optimize file_path,add coroutine rpc api, cmake modify pb
</commit_message>
<xml_diff>
--- a/config/excel/ServerList.xlsx
+++ b/config/excel/ServerList.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proj\server_demo\config\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proj\demo1\config\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B3DFBF-A2FE-4C83-912C-AEA08CE33811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16200" yWindow="408" windowWidth="20448" windowHeight="20592"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ServerList" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,58 +91,62 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>[int32]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ServerIp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务器地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务对外地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PublicIp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127.0.0.1 9997</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络线程数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NetThreadsNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dbSercer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>127.0.0.1 9999</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[int32]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ServerIp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>服务器地址</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>服务对外地址</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PublicIp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>127.0.0.1 9997</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int32</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>网络线程数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NetThreadsNum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -459,25 +464,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -488,19 +493,19 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -514,19 +519,19 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -540,19 +545,19 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10001</v>
       </c>
@@ -566,19 +571,19 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20001</v>
       </c>
@@ -592,13 +597,36 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>30001</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add http address config on serverlist
</commit_message>
<xml_diff>
--- a/config/excel/ServerList.xlsx
+++ b/config/excel/ServerList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proj\demo1\config\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proj\server_demo\config\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5AF3FB-F82D-406A-A068-059BD08756A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BC15C0-E4AE-4210-8EBD-0F93D3279B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -144,6 +144,26 @@
   </si>
   <si>
     <t>127.0.0.1 9990</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTTP线程数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTTP地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HttpIp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127.0.0.1 10097</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HttpThreadsNum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -469,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H7"/>
+  <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -483,10 +503,10 @@
     <col min="5" max="5" width="17.25" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -508,8 +528,14 @@
       <c r="H2" t="s">
         <v>25</v>
       </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -534,8 +560,14 @@
       <c r="H3" t="s">
         <v>24</v>
       </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -560,8 +592,14 @@
       <c r="H4" t="s">
         <v>26</v>
       </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10001</v>
       </c>
@@ -586,8 +624,14 @@
       <c r="H5">
         <v>4</v>
       </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20001</v>
       </c>
@@ -610,7 +654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>30001</v>
       </c>

</xml_diff>

<commit_message>
server connect config remove Gate/Logic connect each other
</commit_message>
<xml_diff>
--- a/config/excel/ServerList.xlsx
+++ b/config/excel/ServerList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15325" windowHeight="4740"/>
+    <workbookView windowWidth="24582" windowHeight="12437"/>
   </bookViews>
   <sheets>
     <sheet name="ServerList" sheetId="1" r:id="rId1"/>
@@ -116,10 +116,10 @@
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,14 +129,136 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,135 +271,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -288,13 +281,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,169 +425,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,80 +472,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -573,157 +492,231 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1046,7 +1039,7 @@
   <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" outlineLevelRow="6"/>
@@ -1200,9 +1193,7 @@
       <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
+      <c r="G6"/>
       <c r="H6">
         <v>2</v>
       </c>

</xml_diff>